<commit_message>
added some values to the schematic as I filled in the BOM
</commit_message>
<xml_diff>
--- a/bom-calculations.xlsx
+++ b/bom-calculations.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="24380" yWindow="2280" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bom-options" sheetId="1" r:id="rId1"/>
     <sheet name="LED" sheetId="2" r:id="rId2"/>
     <sheet name="Costs" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="172">
   <si>
     <t>LED Driver</t>
   </si>
@@ -396,6 +397,147 @@
   </si>
   <si>
     <t>lm317</t>
+  </si>
+  <si>
+    <t>UB-M5BR-DM14</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
+  </si>
+  <si>
+    <t>12 mm Buzzer</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>adafruit</t>
+  </si>
+  <si>
+    <t>arrow</t>
+  </si>
+  <si>
+    <t>sparkfun</t>
+  </si>
+  <si>
+    <t>2.2K 0805 Resistor</t>
+  </si>
+  <si>
+    <t>schematic page</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>reset switch</t>
+  </si>
+  <si>
+    <t>xres pullup 0805 10K</t>
+  </si>
+  <si>
+    <t>CYBLE-014008-00</t>
+  </si>
+  <si>
+    <t>lcd connector</t>
+  </si>
+  <si>
+    <t>mp3 connector</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>455-1721-ND</t>
+  </si>
+  <si>
+    <t>1655-1359-1-ND</t>
+  </si>
+  <si>
+    <t>switch diodes</t>
+  </si>
+  <si>
+    <t>leds</t>
+  </si>
+  <si>
+    <t>mma8452Q</t>
+  </si>
+  <si>
+    <t>accelerometer</t>
+  </si>
+  <si>
+    <t>pca9306</t>
+  </si>
+  <si>
+    <t>i2c level shifter</t>
+  </si>
+  <si>
+    <t>mosfet</t>
+  </si>
+  <si>
+    <t>led resistors - 0805 330Ohm</t>
+  </si>
+  <si>
+    <t>455-1642-ND</t>
+  </si>
+  <si>
+    <t>accel 01 uF 0805 capacitor</t>
+  </si>
+  <si>
+    <t>accel 4.7uF 0805 capcitor</t>
+  </si>
+  <si>
+    <t>MMA8452QR1CT-ND</t>
+  </si>
+  <si>
+    <t>voltage regulator</t>
+  </si>
+  <si>
+    <t>cap 0.1uF 0805</t>
+  </si>
+  <si>
+    <t>cap 1uF 0805</t>
+  </si>
+  <si>
+    <t>resistor 0805 1.8K</t>
+  </si>
+  <si>
+    <t>resistor 0805 1.2K</t>
+  </si>
+  <si>
+    <t>AZ1117CH-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>level pullups 0805 10K</t>
+  </si>
+  <si>
+    <t>DMG1012UW-7DICT-ND</t>
+  </si>
+  <si>
+    <t>capsense resistors 0805 560ohm</t>
+  </si>
+  <si>
+    <t>switches</t>
+  </si>
+  <si>
+    <t>COM-08720</t>
+  </si>
+  <si>
+    <t>PS1240</t>
+  </si>
+  <si>
+    <t>PID:297</t>
+  </si>
+  <si>
+    <t>PID: 820</t>
+  </si>
+  <si>
+    <t>568-4243-1-ND</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -403,9 +545,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -429,6 +571,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -447,7 +597,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -463,13 +613,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -479,6 +638,14 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1485,9 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1523,7 +1688,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <f>F3*G3</f>
+        <f t="shared" ref="B3:B21" si="0">F3*G3</f>
         <v>2.56</v>
       </c>
       <c r="C3" t="s">
@@ -1545,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <f>F4*G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -1566,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <f>F5*G5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C5" t="s">
@@ -1587,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f>F6*G6</f>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="C6" t="s">
@@ -1608,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <f>F7*G7</f>
+        <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
       <c r="C7" t="s">
@@ -1629,7 +1794,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>F8*G8</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="C8" t="s">
@@ -1651,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <f>F9*G9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9" t="s">
@@ -1672,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <f>F10*G10</f>
+        <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
       <c r="C10" t="s">
@@ -1694,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <f>F11*G11</f>
+        <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
       <c r="C11" t="s">
@@ -1717,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <f>F12*G12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C12" t="s">
@@ -1738,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <f>F13*G13</f>
+        <f t="shared" si="0"/>
         <v>2.48</v>
       </c>
       <c r="C13" t="s">
@@ -1762,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <f>F14*G14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C14" t="s">
@@ -1777,7 +1942,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <f>F15*G15</f>
+        <f t="shared" si="0"/>
         <v>1.4850000000000001</v>
       </c>
       <c r="C15" t="s">
@@ -1801,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <f>F16*G16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16" t="s">
@@ -1816,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <f>F17*G17</f>
+        <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
       <c r="C17" t="s">
@@ -1834,7 +1999,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18">
-        <f>F18*G18</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="C18" t="s">
@@ -1855,7 +2020,7 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <f>F19*G19</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C19" t="s">
@@ -1876,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <f>F20*G20</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="C20" t="s">
@@ -1897,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <f>F21*G21</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C21" t="s">
@@ -1938,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <f>F23*G23</f>
+        <f t="shared" ref="B23:B33" si="1">F23*G23</f>
         <v>0</v>
       </c>
       <c r="C23" t="s">
@@ -1959,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <f>F24*G24</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="C24" t="s">
@@ -1980,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <f>F25*G25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C25" t="s">
@@ -2001,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <f>F26*G26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C26" t="s">
@@ -2019,43 +2184,43 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27">
-        <f>F27*G27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="B28">
-        <f>F28*G28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29">
-        <f>F29*G29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30">
-        <f>F30*G30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31">
-        <f>F31*G31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32">
-        <f>F32*G32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33">
-        <f>F33*G33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2068,4 +2233,642 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2">
+        <f t="shared" ref="B2:B9" si="0">C2*D2</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.95</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.21</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10">
+        <f>C10*D10</f>
+        <v>0.34</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.34</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11">
+        <f>C11*D11</f>
+        <v>23.400000000000002</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2.6</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <f>C12*D12</f>
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B26" si="1">C13*D13</f>
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <f>7/25</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>1.28</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1.28</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0.17</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.65</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27">
+        <f>C27*D27</f>
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <f>(9+16)*2</f>
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>0.06</v>
+      </c>
+      <c r="G27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>43.737100000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to the bom
</commit_message>
<xml_diff>
--- a/bom-calculations.xlsx
+++ b/bom-calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="2280" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bom-options" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="174">
   <si>
     <t>LED Driver</t>
   </si>
@@ -538,14 +538,21 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>neward</t>
+  </si>
+  <si>
+    <t>46P5313</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -588,7 +595,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -596,8 +603,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -621,14 +643,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -646,6 +675,9 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2237,9 +2269,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2248,619 +2282,658 @@
     <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" s="3" t="s">
+    <row r="2" spans="1:12">
+      <c r="B2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2">
-        <f t="shared" ref="B2:B9" si="0">C2*D2</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="L2" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" s="5">
+        <f t="shared" ref="B3:B10" si="0">C3*D3</f>
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+      <c r="L3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
         <v>140</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="6">
         <v>1.5</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>140</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="5">
         <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
         <v>140</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="5">
         <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
         <v>140</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="5">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
         <v>0.95</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
         <v>140</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="5">
         <f t="shared" si="0"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>140</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="5">
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
         <v>0.21</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10">
-        <f>C10*D10</f>
-        <v>0.34</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0.34</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>139</v>
-      </c>
-      <c r="H10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>140</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <f>C11*D11</f>
-        <v>23.400000000000002</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>2.6</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>164</v>
-      </c>
-      <c r="I11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>0.34</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.34</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>140</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <f>C12*D12</f>
-        <v>0.70109999999999995</v>
-      </c>
-      <c r="C12">
+        <v>23.400000000000002</v>
+      </c>
+      <c r="C12" s="6">
         <v>9</v>
       </c>
-      <c r="D12">
-        <v>7.7899999999999997E-2</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="E12" s="6">
         <v>3</v>
       </c>
-      <c r="G12" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>140</v>
       </c>
-      <c r="B13">
-        <f t="shared" ref="B13:B26" si="1">C13*D13</f>
+      <c r="B13" s="5">
+        <f>C13*D13</f>
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="C13" s="6">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" ref="B14:B27" si="1">C14*D14</f>
         <v>4.4800000000000004</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="6">
         <v>16</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="6">
         <f>7/25</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="E13">
+      <c r="E14" s="6">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
         <v>140</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="5">
         <f t="shared" si="1"/>
         <v>0.26800000000000002</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="6">
         <v>4</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="6">
         <v>2</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
         <v>140</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="5">
         <f t="shared" si="1"/>
         <v>1.28</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
         <v>1.28</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="6">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="1"/>
-        <v>0.17</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>140</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <f t="shared" si="1"/>
+        <v>0.17</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>4</v>
       </c>
-      <c r="G17" t="s">
-        <v>153</v>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>140</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <f t="shared" si="1"/>
-        <v>0.65</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>0.65</v>
-      </c>
-      <c r="E18">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E18" s="6">
         <v>4</v>
       </c>
-      <c r="F18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G18" t="s">
-        <v>148</v>
-      </c>
-      <c r="H18" t="s">
-        <v>169</v>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>140</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E19">
+        <v>0.65</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="E19" s="6">
         <v>4</v>
       </c>
-      <c r="G19" t="s">
-        <v>149</v>
+      <c r="F19" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="H19" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>140</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <f t="shared" si="1"/>
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E20" s="6">
         <v>4</v>
       </c>
-      <c r="G20" t="s">
-        <v>161</v>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>140</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H21" t="s">
-        <v>160</v>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>140</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <f t="shared" si="1"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="E22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E22" s="6">
         <v>5</v>
       </c>
-      <c r="G22" t="s">
-        <v>156</v>
+      <c r="F22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>140</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <f t="shared" si="1"/>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
-        <v>157</v>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>140</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <f t="shared" si="1"/>
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E24">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E24" s="6">
         <v>5</v>
       </c>
-      <c r="G24" t="s">
-        <v>158</v>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>140</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <f t="shared" si="1"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>5</v>
       </c>
-      <c r="G25" t="s">
-        <v>159</v>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>140</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="G26" t="s">
-        <v>109</v>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>140</v>
       </c>
-      <c r="B27">
-        <f>C27*D27</f>
+      <c r="B27" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="5">
+        <f>C28*D28</f>
         <v>3</v>
       </c>
-      <c r="C27">
+      <c r="C28" s="6">
         <f>(9+16)*2</f>
         <v>50</v>
       </c>
-      <c r="D27">
+      <c r="D28" s="6">
         <v>0.06</v>
       </c>
-      <c r="G27" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="B28">
-        <f>SUM(B2:B27)</f>
-        <v>43.737100000000005</v>
-      </c>
+    <row r="29" spans="1:8">
+      <c r="B29" s="6">
+        <f>SUM(B3:B28)</f>
+        <v>44.079100000000004</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updates to excel sheets with schedule and bom
</commit_message>
<xml_diff>
--- a/bom-calculations.xlsx
+++ b/bom-calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29660" windowHeight="27600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bom-options" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="204">
   <si>
     <t>LED Driver</t>
   </si>
@@ -480,9 +480,6 @@
     <t>455-1642-ND</t>
   </si>
   <si>
-    <t>accel 01 uF 0805 capacitor</t>
-  </si>
-  <si>
     <t>accel 4.7uF 0805 capcitor</t>
   </si>
   <si>
@@ -531,9 +528,6 @@
     <t>PID: 820</t>
   </si>
   <si>
-    <t>568-4243-1-ND</t>
-  </si>
-  <si>
     <t>Wire</t>
   </si>
   <si>
@@ -544,6 +538,102 @@
   </si>
   <si>
     <t>46P5313</t>
+  </si>
+  <si>
+    <t>Motor Hbridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB6612FNGC8ELCT-ND </t>
+  </si>
+  <si>
+    <t>296-17988-1-ND</t>
+  </si>
+  <si>
+    <t>0805 10K</t>
+  </si>
+  <si>
+    <t>0805 560</t>
+  </si>
+  <si>
+    <t>0805 2.2K</t>
+  </si>
+  <si>
+    <t>RMCF0805JT2K20CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT560RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT330RCT-ND</t>
+  </si>
+  <si>
+    <t>311-1361-1-ND</t>
+  </si>
+  <si>
+    <t>490-3335-1-ND</t>
+  </si>
+  <si>
+    <t>311-1365-1-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT1K20CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT1K80CT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-P06J561V</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ122V</t>
+  </si>
+  <si>
+    <t>ERJ-P06J182V</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t>ERJ-P06J222V</t>
+  </si>
+  <si>
+    <t>ERJ-P06J331V</t>
+  </si>
+  <si>
+    <t>TB6612FNG,C,8,EL</t>
+  </si>
+  <si>
+    <t>CC0805ZRY5V9BB104</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>accel 1uF 0805 capacitor</t>
+  </si>
+  <si>
+    <t>GRM21BR61E475KA12L</t>
+  </si>
+  <si>
+    <t>PCA9306DCUR</t>
+  </si>
+  <si>
+    <t>DMG1012UW-7</t>
+  </si>
+  <si>
+    <t>AZ1117CH-3.3TRG1</t>
+  </si>
+  <si>
+    <t>MMA8452QR1</t>
+  </si>
+  <si>
+    <t>S4B-PH-K-S(LF)(SN)</t>
+  </si>
+  <si>
+    <t>B5P-VH(LF)(SN)</t>
   </si>
 </sst>
 </file>
@@ -619,7 +709,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,6 +720,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -657,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -678,6 +784,22 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2269,10 +2391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L29"/>
+  <dimension ref="A2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2290,7 +2412,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>133</v>
@@ -2312,7 +2434,7 @@
         <v>131</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2336,7 +2458,7 @@
         <v>126</v>
       </c>
       <c r="L3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2361,7 +2483,7 @@
         <v>127</v>
       </c>
       <c r="I4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2381,9 +2503,17 @@
       <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>177</v>
+      </c>
       <c r="G5" s="6" t="s">
         <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2403,9 +2533,17 @@
       <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="G6" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="H6" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2430,7 +2568,7 @@
         <v>135</v>
       </c>
       <c r="K7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2450,9 +2588,17 @@
       <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G8" s="6" t="s">
         <v>136</v>
+      </c>
+      <c r="H8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J8" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2499,6 +2645,9 @@
       <c r="H10" t="s">
         <v>141</v>
       </c>
+      <c r="J10" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
@@ -2524,6 +2673,9 @@
       <c r="H11" t="s">
         <v>151</v>
       </c>
+      <c r="J11" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
@@ -2544,10 +2696,10 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2580,7 +2732,7 @@
         <v>140</v>
       </c>
       <c r="B14" s="5">
-        <f t="shared" ref="B14:B27" si="1">C14*D14</f>
+        <f t="shared" ref="B14:B28" si="1">C14*D14</f>
         <v>4.4800000000000004</v>
       </c>
       <c r="C14" s="6">
@@ -2598,7 +2750,7 @@
         <v>144</v>
       </c>
       <c r="I14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2622,6 +2774,12 @@
       <c r="G15" s="6" t="s">
         <v>150</v>
       </c>
+      <c r="H15" t="s">
+        <v>181</v>
+      </c>
+      <c r="J15" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
@@ -2647,10 +2805,13 @@
         <v>146</v>
       </c>
       <c r="H16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>153</v>
+      </c>
+      <c r="J16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -2669,10 +2830,16 @@
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>196</v>
+      </c>
+      <c r="H17" t="s">
+        <v>182</v>
+      </c>
+      <c r="J17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -2691,22 +2858,28 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>152</v>
+      </c>
+      <c r="H18" t="s">
+        <v>183</v>
+      </c>
+      <c r="J18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>140</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
       <c r="D19" s="6">
-        <v>0.65</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="E19" s="6">
         <v>4</v>
@@ -2718,10 +2891,13 @@
         <v>148</v>
       </c>
       <c r="H19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>174</v>
+      </c>
+      <c r="J19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -2743,10 +2919,13 @@
         <v>149</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>161</v>
+      </c>
+      <c r="J20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -2765,10 +2944,16 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>160</v>
+      </c>
+      <c r="H21" t="s">
+        <v>180</v>
+      </c>
+      <c r="J21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -2789,13 +2974,16 @@
         <v>124</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>159</v>
+      </c>
+      <c r="J22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -2814,10 +3002,16 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>155</v>
+      </c>
+      <c r="H23" t="s">
+        <v>182</v>
+      </c>
+      <c r="J23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -2836,10 +3030,16 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>156</v>
+      </c>
+      <c r="H24" t="s">
+        <v>184</v>
+      </c>
+      <c r="J24" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -2858,10 +3058,16 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>157</v>
+      </c>
+      <c r="H25" t="s">
+        <v>186</v>
+      </c>
+      <c r="J25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -2880,60 +3086,91 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>140</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="H26" t="s">
+        <v>185</v>
+      </c>
+      <c r="J26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="B27" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1.27</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
       <c r="D27" s="6">
-        <v>4</v>
-      </c>
-      <c r="E27" s="6"/>
+        <v>1.27</v>
+      </c>
+      <c r="E27" s="6">
+        <v>6</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>172</v>
+      </c>
+      <c r="H27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>140</v>
       </c>
       <c r="B28" s="5">
-        <f>C28*D28</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="C28" s="6">
-        <f>(9+16)*2</f>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D28" s="6">
-        <v>0.06</v>
+        <v>4</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="B29" s="6">
-        <f>SUM(B3:B28)</f>
-        <v>44.079100000000004</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="5">
+        <f>C29*D29</f>
+        <v>3</v>
+      </c>
+      <c r="C29" s="6">
+        <f>(9+16)*2</f>
+        <v>50</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.06</v>
+      </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="6">
+        <f>SUM(B3:B29)</f>
+        <v>45.393100000000011</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Released version 1.2 of board
</commit_message>
<xml_diff>
--- a/bom-calculations.xlsx
+++ b/bom-calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bom-options" sheetId="1" r:id="rId1"/>
@@ -2481,7 +2481,7 @@
   <dimension ref="A2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2718,14 +2718,14 @@
     <row r="10" spans="1:13">
       <c r="A10" s="9">
         <f>B10</f>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="6">
         <v>0.21</v>
@@ -2748,10 +2748,10 @@
     <row r="11" spans="1:13">
       <c r="B11" s="5">
         <f>C11*D11</f>
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="C11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="6">
         <v>0.34</v>
@@ -2960,14 +2960,14 @@
     <row r="19" spans="1:11">
       <c r="A19" s="9">
         <f>B19</f>
-        <v>0.69399999999999995</v>
+        <v>0</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" si="1"/>
-        <v>0.69399999999999995</v>
+        <v>0</v>
       </c>
       <c r="C19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="6">
         <v>0.69399999999999995</v>
@@ -2994,14 +2994,14 @@
     <row r="20" spans="1:11">
       <c r="A20" s="9">
         <f>B20</f>
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="6">
         <v>0.14000000000000001</v>
@@ -3026,14 +3026,14 @@
     <row r="21" spans="1:11">
       <c r="A21" s="9">
         <f>B21</f>
-        <v>0.13400000000000001</v>
+        <v>0</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" si="1"/>
-        <v>0.13400000000000001</v>
+        <v>0</v>
       </c>
       <c r="C21" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="6">
         <v>6.7000000000000004E-2</v>
@@ -3224,13 +3224,13 @@
     <row r="28" spans="1:11">
       <c r="B28" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
       <c r="D28" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3261,7 +3261,7 @@
     <row r="30" spans="1:11">
       <c r="B30" s="6">
         <f>SUM(B3:B29)</f>
-        <v>43.727000000000011</v>
+        <v>43.20900000000001</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>

</xml_diff>

<commit_message>
a bunch of changes to the test firmware
</commit_message>
<xml_diff>
--- a/bom-calculations.xlsx
+++ b/bom-calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28320" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bom-options" sheetId="1" r:id="rId1"/>
@@ -2480,8 +2480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2527,7 +2527,8 @@
     </row>
     <row r="3" spans="1:13">
       <c r="B3" s="5">
-        <v>0.94399999999999995</v>
+        <f>C3*D3</f>
+        <v>0.34200000000000003</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -2553,7 +2554,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="B4" s="5">
-        <f t="shared" ref="B4:B10" si="0">C4*D4</f>
+        <f t="shared" ref="B4:B29" si="0">C4*D4</f>
         <v>1.008</v>
       </c>
       <c r="C4" s="6">
@@ -2747,7 +2748,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="5">
-        <f>C11*D11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11" s="6">
@@ -2773,7 +2774,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="5">
-        <f>C12*D12</f>
+        <f t="shared" si="0"/>
         <v>23.400000000000002</v>
       </c>
       <c r="C12" s="6">
@@ -2796,7 +2797,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="5">
-        <f>C13*D13</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="C13" s="6">
@@ -2821,7 +2822,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="5">
-        <f t="shared" ref="B14:B28" si="1">C14*D14</f>
+        <f t="shared" si="0"/>
         <v>4.4800000000000004</v>
       </c>
       <c r="C14" s="6">
@@ -2845,7 +2846,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.26800000000000002</v>
       </c>
       <c r="C15" s="6">
@@ -2873,7 +2874,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
       <c r="C16" s="6">
@@ -2903,7 +2904,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="B17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
       <c r="C17" s="6">
@@ -2931,7 +2932,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="B18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C18" s="6">
@@ -2963,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C19" s="6">
@@ -2997,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C20" s="6">
@@ -3029,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C21" s="6">
@@ -3057,7 +3058,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="B22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="C22" s="6">
@@ -3085,7 +3086,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="B23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C23" s="6">
@@ -3113,7 +3114,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="B24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C24" s="6">
@@ -3141,7 +3142,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="B25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C25" s="6">
@@ -3169,7 +3170,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="B26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C26" s="6">
@@ -3197,7 +3198,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="B27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.27</v>
       </c>
       <c r="C27" s="6">
@@ -3223,7 +3224,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="B28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C28" s="6">
@@ -3241,7 +3242,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="B29" s="5">
-        <f>C29*D29</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C29" s="6">
@@ -3259,9 +3260,9 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <f>SUM(B3:B29)</f>
-        <v>43.20900000000001</v>
+        <v>42.607000000000006</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>

</xml_diff>